<commit_message>
Penambahan informasi diskon di module ImportExportData golongan dan produk
</commit_message>
<xml_diff>
--- a/format file import/File Import Excel/Master Data/data_golongan.xlsx
+++ b/format file import/File Import Excel/Master Data/data_golongan.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>KETERANGAN INPUT DATA MELALUI EXCEL</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Jika melanggar ketentuan di atas, proses import data akan gagal</t>
+  </si>
+  <si>
+    <t>DISKON</t>
   </si>
 </sst>
 </file>
@@ -131,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -152,6 +155,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -454,20 +460,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.28515625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -481,7 +490,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Penambahan input persentasi margin keuntungan di module golongan untuk menentukan harga jual otomatis pada saat input produk
</commit_message>
<xml_diff>
--- a/format file import/File Import Excel/Master Data/data_golongan.xlsx
+++ b/format file import/File Import Excel/Master Data/data_golongan.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>KETERANGAN INPUT DATA MELALUI EXCEL</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>DISKON</t>
+  </si>
+  <si>
+    <t>KEUNTUNGAN (%)</t>
   </si>
 </sst>
 </file>
@@ -153,11 +156,11 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -460,22 +463,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -490,7 +497,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,10 +507,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>

</xml_diff>